<commit_message>
Atualização: novo formato de planilha
</commit_message>
<xml_diff>
--- a/finanplan-2025.xlsx
+++ b/finanplan-2025.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="579"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="579" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Informações" sheetId="1" r:id="rId1"/>
@@ -2822,12 +2822,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="113068288"/>
-        <c:axId val="113070080"/>
+        <c:axId val="122439936"/>
+        <c:axId val="122441728"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="113068288"/>
+        <c:axId val="122439936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2858,14 +2858,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113070080"/>
+        <c:crossAx val="122441728"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113070080"/>
+        <c:axId val="122441728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2873,7 +2873,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113068288"/>
+        <c:crossAx val="122439936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2889,7 +2889,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3067,12 +3067,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="113111040"/>
-        <c:axId val="113112576"/>
+        <c:axId val="122478592"/>
+        <c:axId val="122480128"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="113111040"/>
+        <c:axId val="122478592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3103,14 +3103,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113112576"/>
+        <c:crossAx val="122480128"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113112576"/>
+        <c:axId val="122480128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3118,7 +3118,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113111040"/>
+        <c:crossAx val="122478592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3134,7 +3134,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3312,12 +3312,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="110515712"/>
-        <c:axId val="110517248"/>
+        <c:axId val="122045952"/>
+        <c:axId val="122047488"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="110515712"/>
+        <c:axId val="122045952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3348,14 +3348,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110517248"/>
+        <c:crossAx val="122047488"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110517248"/>
+        <c:axId val="122047488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3363,7 +3363,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110515712"/>
+        <c:crossAx val="122045952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3379,7 +3379,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3396,10 +3396,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="3.1782889485523609E-2"/>
-          <c:y val="0.14179691892499705"/>
-          <c:w val="0.94448878891227062"/>
-          <c:h val="0.65883278983470184"/>
+          <c:x val="3.1782889485523616E-2"/>
+          <c:y val="0.14179691892499707"/>
+          <c:w val="0.94448878891227039"/>
+          <c:h val="0.65883278983470173"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3567,12 +3567,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:dPt>
-            <c:idx val="9"/>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="11"/>
-          </c:dPt>
           <c:dLbls>
             <c:txPr>
               <a:bodyPr rot="-2640000" wrap="none"/>
@@ -3691,11 +3685,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="113586944"/>
-        <c:axId val="113588480"/>
+        <c:axId val="122892288"/>
+        <c:axId val="122893824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113586944"/>
+        <c:axId val="122892288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3726,14 +3720,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113588480"/>
+        <c:crossAx val="122893824"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113588480"/>
+        <c:axId val="122893824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3741,7 +3735,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113586944"/>
+        <c:crossAx val="122892288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3758,9 +3752,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.7731397342957795E-2"/>
-          <c:y val="1.5618493199569294E-2"/>
-          <c:w val="0.15346318773166712"/>
+          <c:x val="2.7731397342957799E-2"/>
+          <c:y val="1.5618493199569296E-2"/>
+          <c:w val="0.1534631877316672"/>
           <c:h val="7.2238275172260516E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3799,7 +3793,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6776,7 +6770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
@@ -7064,7 +7058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AML23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
@@ -12504,7 +12498,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1"/>
@@ -16055,8 +16049,8 @@
   <dimension ref="A1:XFD1033"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1"/>
@@ -19822,7 +19816,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1"/>
@@ -48045,7 +48039,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1"/>
@@ -50356,9 +50350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1"/>
   <cols>

</xml_diff>